<commit_message>
New walk forward, added early stop to hyperparameter tuning
</commit_message>
<xml_diff>
--- a/Metrics/NewTestingMetrics.xlsx
+++ b/Metrics/NewTestingMetrics.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.261</v>
+        <v>0.252</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.066</v>
+        <v>-0.079</v>
       </c>
       <c r="D3" t="n">
-        <v>0.469</v>
+        <v>0.474</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6850000000000001</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="F3" t="n">
-        <v>0.769</v>
+        <v>0.786</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5570000000000001</v>
+        <v>0.5649999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.193</v>
+        <v>0.119</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.164</v>
+        <v>-0.271</v>
       </c>
       <c r="D4" t="n">
-        <v>0.512</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>0.716</v>
+        <v>0.748</v>
       </c>
       <c r="F4" t="n">
-        <v>0.741</v>
+        <v>0.771</v>
       </c>
       <c r="G4" t="n">
-        <v>0.501</v>
+        <v>0.467</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,47 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.157</v>
+        <v>0.016</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.041</v>
+        <v>-0.216</v>
       </c>
       <c r="D5" t="n">
-        <v>0.481</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>0.694</v>
+        <v>0.749</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.731</v>
       </c>
       <c r="G5" t="n">
-        <v>0.555</v>
+        <v>0.452</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Ensemble</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.293</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.697</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated walk forward validation, some updated code for running on server
</commit_message>
<xml_diff>
--- a/Metrics/NewTestingMetrics.xlsx
+++ b/Metrics/NewTestingMetrics.xlsx
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.252</v>
+        <v>0.243</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.079</v>
+        <v>-0.092</v>
       </c>
       <c r="D3" t="n">
-        <v>0.474</v>
+        <v>0.48</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="F3" t="n">
-        <v>0.786</v>
+        <v>0.769</v>
       </c>
       <c r="G3" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.545</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.119</v>
+        <v>0.258</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.271</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.471</v>
       </c>
       <c r="E4" t="n">
-        <v>0.748</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>0.771</v>
+        <v>0.751</v>
       </c>
       <c r="G4" t="n">
-        <v>0.467</v>
+        <v>0.545</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.016</v>
+        <v>0.024</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.216</v>
+        <v>-0.206</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.556</v>
       </c>
       <c r="E5" t="n">
-        <v>0.749</v>
+        <v>0.746</v>
       </c>
       <c r="F5" t="n">
-        <v>0.731</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>0.452</v>
+        <v>0.336</v>
       </c>
     </row>
     <row r="6">
@@ -572,22 +572,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.293</v>
+        <v>0.296</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.02</v>
+        <v>-0.015</v>
       </c>
       <c r="D6" t="n">
-        <v>0.448</v>
+        <v>0.447</v>
       </c>
       <c r="E6" t="n">
         <v>0.669</v>
       </c>
       <c r="F6" t="n">
-        <v>0.697</v>
+        <v>0.679</v>
       </c>
       <c r="G6" t="n">
-        <v>0.544</v>
+        <v>0.546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>